<commit_message>
Update to latest indices and docs
</commit_message>
<xml_diff>
--- a/Outputs/Performance of example MPs.xlsx
+++ b/Outputs/Performance of example MPs.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\abft-mse\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="For publication" sheetId="3" r:id="rId1"/>
     <sheet name="raw East_perf" sheetId="1" r:id="rId2"/>
     <sheet name="raw West_perf" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -604,12 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -617,10 +611,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -942,21 +942,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="16" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="12" width="6.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.109375" style="1" customWidth="1"/>
+    <col min="15" max="16" width="6.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
@@ -973,103 +976,103 @@
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
     </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-    </row>
-    <row r="3" spans="2:16" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-    </row>
-    <row r="4" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" spans="2:16" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="str">
+      <c r="C4" s="11"/>
+      <c r="D4" s="8" t="str">
         <f>'raw East_perf'!B1</f>
         <v>C10</v>
       </c>
-      <c r="E4" s="11" t="str">
+      <c r="E4" s="8" t="str">
         <f>'raw East_perf'!C1</f>
         <v>C20</v>
       </c>
-      <c r="F4" s="11" t="str">
+      <c r="F4" s="8" t="str">
         <f>'raw East_perf'!D1</f>
         <v>C30</v>
       </c>
-      <c r="G4" s="11" t="str">
+      <c r="G4" s="8" t="str">
         <f>'raw East_perf'!E1</f>
         <v>D10</v>
       </c>
-      <c r="H4" s="11" t="str">
+      <c r="H4" s="8" t="str">
         <f>'raw East_perf'!F1</f>
         <v>D20</v>
       </c>
-      <c r="I4" s="11" t="str">
+      <c r="I4" s="8" t="str">
         <f>'raw East_perf'!G1</f>
         <v>D30</v>
       </c>
-      <c r="J4" s="11" t="str">
+      <c r="J4" s="8" t="str">
         <f>'raw East_perf'!H1</f>
         <v>LD</v>
       </c>
-      <c r="K4" s="11" t="str">
+      <c r="K4" s="8" t="str">
         <f>'raw East_perf'!I1</f>
         <v>DNC</v>
       </c>
-      <c r="L4" s="11" t="str">
+      <c r="L4" s="8" t="str">
         <f>'raw East_perf'!J1</f>
         <v>LDNC</v>
       </c>
-      <c r="M4" s="11" t="str">
+      <c r="M4" s="8" t="str">
         <f>'raw East_perf'!K1</f>
         <v>POF</v>
       </c>
-      <c r="N4" s="11" t="str">
+      <c r="N4" s="8" t="str">
         <f>'raw East_perf'!L1</f>
         <v>POS</v>
       </c>
-      <c r="O4" s="11" t="str">
+      <c r="O4" s="8" t="str">
         <f>'raw East_perf'!M1</f>
         <v>PGK</v>
       </c>
-      <c r="P4" s="11" t="str">
+      <c r="P4" s="8" t="str">
         <f>'raw East_perf'!N1</f>
         <v>AAVC</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C5" t="str">
         <f>'raw East_perf'!A2</f>
         <v>ZeroC-ZeroC</v>
@@ -1088,19 +1091,19 @@
       </c>
       <c r="G5" s="2">
         <f>'raw East_perf'!E2</f>
-        <v>0.55400000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="H5" s="2">
         <f>'raw East_perf'!F2</f>
-        <v>0.76</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="I5" s="2">
         <f>'raw East_perf'!G2</f>
-        <v>0.85299999999999998</v>
+        <v>0.82099999999999995</v>
       </c>
       <c r="J5" s="2">
         <f>'raw East_perf'!H2</f>
-        <v>0.432</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="K5" s="2">
         <f>'raw East_perf'!I2</f>
@@ -1124,49 +1127,49 @@
       </c>
       <c r="P5" s="2">
         <f>'raw East_perf'!N2</f>
-        <v>1.948</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+        <v>1.7030000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C6" t="str">
         <f>'raw East_perf'!A3</f>
         <v>CurC50-CurC50</v>
       </c>
       <c r="D6" s="2">
         <f>'raw East_perf'!B3</f>
-        <v>6.024</v>
+        <v>5.8970000000000002</v>
       </c>
       <c r="E6" s="2">
         <f>'raw East_perf'!C3</f>
-        <v>5.83</v>
+        <v>5.8970000000000002</v>
       </c>
       <c r="F6" s="2">
         <f>'raw East_perf'!D3</f>
-        <v>5.96</v>
+        <v>5.8970000000000002</v>
       </c>
       <c r="G6" s="2">
         <f>'raw East_perf'!E3</f>
-        <v>0.51200000000000001</v>
+        <v>0.42</v>
       </c>
       <c r="H6" s="2">
         <f>'raw East_perf'!F3</f>
-        <v>0.66300000000000003</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="I6" s="2">
         <f>'raw East_perf'!G3</f>
-        <v>0.72599999999999998</v>
+        <v>0.71</v>
       </c>
       <c r="J6" s="2">
         <f>'raw East_perf'!H3</f>
-        <v>0.42199999999999999</v>
+        <v>0.316</v>
       </c>
       <c r="K6" s="2">
         <f>'raw East_perf'!I3</f>
-        <v>0.83799999999999997</v>
+        <v>0.85</v>
       </c>
       <c r="L6" s="2">
         <f>'raw East_perf'!J3</f>
-        <v>0.82899999999999996</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="M6" s="2">
         <f>'raw East_perf'!K3</f>
@@ -1182,49 +1185,49 @@
       </c>
       <c r="P6" s="2">
         <f>'raw East_perf'!N3</f>
-        <v>0.41499999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C7" t="str">
         <f>'raw East_perf'!A4</f>
         <v>CurC100-CurC100</v>
       </c>
       <c r="D7" s="2">
         <f>'raw East_perf'!B4</f>
-        <v>11.991</v>
+        <v>11.792999999999999</v>
       </c>
       <c r="E7" s="2">
         <f>'raw East_perf'!C4</f>
-        <v>11.644</v>
+        <v>11.792999999999999</v>
       </c>
       <c r="F7" s="2">
         <f>'raw East_perf'!D4</f>
-        <v>11.91</v>
+        <v>11.792999999999999</v>
       </c>
       <c r="G7" s="2">
         <f>'raw East_perf'!E4</f>
-        <v>0.47099999999999997</v>
+        <v>0.39</v>
       </c>
       <c r="H7" s="2">
         <f>'raw East_perf'!F4</f>
-        <v>0.56200000000000006</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="I7" s="2">
         <f>'raw East_perf'!G4</f>
-        <v>0.59199999999999997</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="J7" s="2">
         <f>'raw East_perf'!H4</f>
-        <v>0.40500000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="K7" s="2">
         <f>'raw East_perf'!I4</f>
-        <v>0.66100000000000003</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="L7" s="2">
         <f>'raw East_perf'!J4</f>
-        <v>0.64400000000000002</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="M7" s="2">
         <f>'raw East_perf'!K4</f>
@@ -1240,49 +1243,49 @@
       </c>
       <c r="P7" s="2">
         <f>'raw East_perf'!N4</f>
-        <v>0.42499999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C8" t="str">
         <f>'raw East_perf'!A5</f>
         <v>CurC150-CurC150</v>
       </c>
       <c r="D8" s="2">
         <f>'raw East_perf'!B5</f>
-        <v>17.902000000000001</v>
+        <v>17.690000000000001</v>
       </c>
       <c r="E8" s="2">
         <f>'raw East_perf'!C5</f>
-        <v>17.34</v>
+        <v>17.690000000000001</v>
       </c>
       <c r="F8" s="2">
         <f>'raw East_perf'!D5</f>
-        <v>17.731000000000002</v>
+        <v>17.690000000000001</v>
       </c>
       <c r="G8" s="2">
         <f>'raw East_perf'!E5</f>
-        <v>0.42899999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="H8" s="2">
         <f>'raw East_perf'!F5</f>
-        <v>0.45900000000000002</v>
+        <v>0.434</v>
       </c>
       <c r="I8" s="2">
         <f>'raw East_perf'!G5</f>
-        <v>0.44600000000000001</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="J8" s="2">
         <f>'raw East_perf'!H5</f>
-        <v>0.32500000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="K8" s="2">
         <f>'raw East_perf'!I5</f>
-        <v>0.44700000000000001</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="L8" s="2">
         <f>'raw East_perf'!J5</f>
-        <v>0.42899999999999999</v>
+        <v>0.495</v>
       </c>
       <c r="M8" s="2">
         <f>'raw East_perf'!K5</f>
@@ -1290,57 +1293,57 @@
       </c>
       <c r="N8" s="2">
         <f>'raw East_perf'!L5</f>
-        <v>6.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="O8" s="2">
         <f>'raw East_perf'!M5</f>
-        <v>99.707999999999998</v>
+        <v>99.91</v>
       </c>
       <c r="P8" s="2">
         <f>'raw East_perf'!N5</f>
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C9" t="str">
         <f>'raw East_perf'!A6</f>
         <v>EMP1e-EMP1w</v>
       </c>
       <c r="D9" s="2">
         <f>'raw East_perf'!B6</f>
-        <v>12.595000000000001</v>
+        <v>12.279</v>
       </c>
       <c r="E9" s="2">
         <f>'raw East_perf'!C6</f>
-        <v>14.53</v>
+        <v>15.244999999999999</v>
       </c>
       <c r="F9" s="2">
         <f>'raw East_perf'!D6</f>
-        <v>18.193999999999999</v>
+        <v>20.606999999999999</v>
       </c>
       <c r="G9" s="2">
         <f>'raw East_perf'!E6</f>
-        <v>0.46899999999999997</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="H9" s="2">
         <f>'raw East_perf'!F6</f>
-        <v>0.54200000000000004</v>
+        <v>0.501</v>
       </c>
       <c r="I9" s="2">
         <f>'raw East_perf'!G6</f>
-        <v>0.52300000000000002</v>
+        <v>0.53</v>
       </c>
       <c r="J9" s="2">
         <f>'raw East_perf'!H6</f>
-        <v>0.28199999999999997</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="K9" s="2">
         <f>'raw East_perf'!I6</f>
-        <v>0.34499999999999997</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="L9" s="2">
         <f>'raw East_perf'!J6</f>
-        <v>0.33600000000000002</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="M9" s="2">
         <f>'raw East_perf'!K6</f>
@@ -1356,49 +1359,49 @@
       </c>
       <c r="P9" s="2">
         <f>'raw East_perf'!N6</f>
-        <v>1.9279999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+        <v>2.238</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C10" t="str">
         <f>'raw East_perf'!A7</f>
         <v>EMP2e-EMP2w</v>
       </c>
       <c r="D10" s="2">
         <f>'raw East_perf'!B7</f>
-        <v>8.6890000000000001</v>
+        <v>12.087</v>
       </c>
       <c r="E10" s="2">
         <f>'raw East_perf'!C7</f>
-        <v>5.3630000000000004</v>
+        <v>13.739000000000001</v>
       </c>
       <c r="F10" s="2">
         <f>'raw East_perf'!D7</f>
-        <v>3.5939999999999999</v>
+        <v>17.321999999999999</v>
       </c>
       <c r="G10" s="2">
         <f>'raw East_perf'!E7</f>
-        <v>0.48699999999999999</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="H10" s="2">
         <f>'raw East_perf'!F7</f>
-        <v>0.63300000000000001</v>
+        <v>0.50700000000000001</v>
       </c>
       <c r="I10" s="2">
         <f>'raw East_perf'!G7</f>
-        <v>0.72499999999999998</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="J10" s="2">
         <f>'raw East_perf'!H7</f>
-        <v>0.41499999999999998</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="K10" s="2">
         <f>'raw East_perf'!I7</f>
-        <v>0.93</v>
+        <v>0.438</v>
       </c>
       <c r="L10" s="2">
         <f>'raw East_perf'!J7</f>
-        <v>0.82299999999999995</v>
+        <v>0.438</v>
       </c>
       <c r="M10" s="2">
         <f>'raw East_perf'!K7</f>
@@ -1414,69 +1417,69 @@
       </c>
       <c r="P10" s="2">
         <f>'raw East_perf'!N7</f>
-        <v>3.927</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+        <v>1.6519999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11" t="str">
+      <c r="C12" s="11"/>
+      <c r="D12" s="8" t="str">
         <f>'raw West_perf'!B1</f>
         <v>C10</v>
       </c>
-      <c r="E12" s="11" t="str">
+      <c r="E12" s="8" t="str">
         <f>'raw West_perf'!C1</f>
         <v>C20</v>
       </c>
-      <c r="F12" s="11" t="str">
+      <c r="F12" s="8" t="str">
         <f>'raw West_perf'!D1</f>
         <v>C30</v>
       </c>
-      <c r="G12" s="11" t="str">
+      <c r="G12" s="8" t="str">
         <f>'raw West_perf'!E1</f>
         <v>D10</v>
       </c>
-      <c r="H12" s="11" t="str">
+      <c r="H12" s="8" t="str">
         <f>'raw West_perf'!F1</f>
         <v>D20</v>
       </c>
-      <c r="I12" s="11" t="str">
+      <c r="I12" s="8" t="str">
         <f>'raw West_perf'!G1</f>
         <v>D30</v>
       </c>
-      <c r="J12" s="11" t="str">
+      <c r="J12" s="8" t="str">
         <f>'raw West_perf'!H1</f>
         <v>LD</v>
       </c>
-      <c r="K12" s="11" t="str">
+      <c r="K12" s="8" t="str">
         <f>'raw West_perf'!I1</f>
         <v>DNC</v>
       </c>
-      <c r="L12" s="11" t="str">
+      <c r="L12" s="8" t="str">
         <f>'raw West_perf'!J1</f>
         <v>LDNC</v>
       </c>
-      <c r="M12" s="11" t="str">
+      <c r="M12" s="8" t="str">
         <f>'raw West_perf'!K1</f>
         <v>POF</v>
       </c>
-      <c r="N12" s="11" t="str">
+      <c r="N12" s="8" t="str">
         <f>'raw West_perf'!L1</f>
         <v>POS</v>
       </c>
-      <c r="O12" s="11" t="str">
+      <c r="O12" s="8" t="str">
         <f>'raw West_perf'!M1</f>
         <v>PGK</v>
       </c>
-      <c r="P12" s="11" t="str">
+      <c r="P12" s="8" t="str">
         <f>'raw West_perf'!N1</f>
         <v>AAVC</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C13" t="str">
         <f>'raw West_perf'!A2</f>
         <v>ZeroC-ZeroC</v>
@@ -1495,19 +1498,19 @@
       </c>
       <c r="G13" s="3">
         <f>'raw West_perf'!E2</f>
-        <v>0.80300000000000005</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="H13" s="3">
         <f>'raw West_perf'!F2</f>
-        <v>1.1950000000000001</v>
+        <v>1.093</v>
       </c>
       <c r="I13" s="3">
         <f>'raw West_perf'!G2</f>
-        <v>1.0760000000000001</v>
+        <v>1.081</v>
       </c>
       <c r="J13" s="3">
         <f>'raw West_perf'!H2</f>
-        <v>0.42</v>
+        <v>0.377</v>
       </c>
       <c r="K13" s="3">
         <f>'raw West_perf'!I2</f>
@@ -1531,49 +1534,49 @@
       </c>
       <c r="P13" s="3">
         <f>'raw West_perf'!N2</f>
-        <v>2.726</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+        <v>1.7030000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C14" t="str">
         <f>'raw West_perf'!A3</f>
         <v>CurC50-CurC50</v>
       </c>
       <c r="D14" s="3">
         <f>'raw West_perf'!B3</f>
-        <v>1.6830000000000001</v>
+        <v>1.8120000000000001</v>
       </c>
       <c r="E14" s="3">
         <f>'raw West_perf'!C3</f>
-        <v>1.8819999999999999</v>
+        <v>1.8140000000000001</v>
       </c>
       <c r="F14" s="3">
         <f>'raw West_perf'!D3</f>
-        <v>1.752</v>
+        <v>1.8140000000000001</v>
       </c>
       <c r="G14" s="3">
         <f>'raw West_perf'!E3</f>
-        <v>0.73899999999999999</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="H14" s="3">
         <f>'raw West_perf'!F3</f>
-        <v>1.0369999999999999</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="I14" s="3">
         <f>'raw West_perf'!G3</f>
-        <v>0.89500000000000002</v>
+        <v>0.876</v>
       </c>
       <c r="J14" s="3">
         <f>'raw West_perf'!H3</f>
-        <v>0.40600000000000003</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="K14" s="3">
         <f>'raw West_perf'!I3</f>
-        <v>0.80400000000000005</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="L14" s="3">
         <f>'raw West_perf'!J3</f>
-        <v>0.79400000000000004</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="M14" s="3">
         <f>'raw West_perf'!K3</f>
@@ -1589,49 +1592,49 @@
       </c>
       <c r="P14" s="3">
         <f>'raw West_perf'!N3</f>
-        <v>1.4570000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
         <f>'raw West_perf'!A4</f>
         <v>CurC100-CurC100</v>
       </c>
       <c r="D15" s="3">
         <f>'raw West_perf'!B4</f>
-        <v>3.2109999999999999</v>
+        <v>3.419</v>
       </c>
       <c r="E15" s="3">
         <f>'raw West_perf'!C4</f>
-        <v>3.7269999999999999</v>
+        <v>3.5979999999999999</v>
       </c>
       <c r="F15" s="3">
         <f>'raw West_perf'!D4</f>
-        <v>3.3980000000000001</v>
+        <v>3.5840000000000001</v>
       </c>
       <c r="G15" s="3">
         <f>'raw West_perf'!E4</f>
-        <v>0.68200000000000005</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="H15" s="3">
         <f>'raw West_perf'!F4</f>
-        <v>0.89</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="I15" s="3">
         <f>'raw West_perf'!G4</f>
-        <v>0.72399999999999998</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="J15" s="3">
         <f>'raw West_perf'!H4</f>
-        <v>0.38600000000000001</v>
+        <v>0.318</v>
       </c>
       <c r="K15" s="3">
         <f>'raw West_perf'!I4</f>
-        <v>0.61499999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="L15" s="3">
         <f>'raw West_perf'!J4</f>
-        <v>0.59799999999999998</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="M15" s="3">
         <f>'raw West_perf'!K4</f>
@@ -1647,49 +1650,49 @@
       </c>
       <c r="P15" s="3">
         <f>'raw West_perf'!N4</f>
-        <v>1.917</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C16" t="str">
         <f>'raw West_perf'!A5</f>
         <v>CurC150-CurC150</v>
       </c>
       <c r="D16" s="3">
         <f>'raw West_perf'!B5</f>
-        <v>4.5960000000000001</v>
+        <v>4.8310000000000004</v>
       </c>
       <c r="E16" s="3">
         <f>'raw West_perf'!C5</f>
-        <v>5.3289999999999997</v>
+        <v>5.0229999999999997</v>
       </c>
       <c r="F16" s="3">
         <f>'raw West_perf'!D5</f>
-        <v>4.7969999999999997</v>
+        <v>4.9489999999999998</v>
       </c>
       <c r="G16" s="3">
         <f>'raw West_perf'!E5</f>
-        <v>0.628</v>
+        <v>0.378</v>
       </c>
       <c r="H16" s="3">
         <f>'raw West_perf'!F5</f>
-        <v>0.75</v>
+        <v>0.627</v>
       </c>
       <c r="I16" s="3">
         <f>'raw West_perf'!G5</f>
-        <v>0.56100000000000005</v>
+        <v>0.501</v>
       </c>
       <c r="J16" s="3">
         <f>'raw West_perf'!H5</f>
-        <v>0.32100000000000001</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="K16" s="3">
         <f>'raw West_perf'!I5</f>
-        <v>0.41899999999999998</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="L16" s="3">
         <f>'raw West_perf'!J5</f>
-        <v>0.39900000000000002</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="M16" s="3">
         <f>'raw West_perf'!K5</f>
@@ -1697,57 +1700,57 @@
       </c>
       <c r="N16" s="3">
         <f>'raw West_perf'!L5</f>
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="O16" s="3">
         <f>'raw West_perf'!M5</f>
-        <v>100</v>
+        <v>99.82</v>
       </c>
       <c r="P16" s="3">
         <f>'raw West_perf'!N5</f>
-        <v>2.2549999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C17" t="str">
         <f>'raw West_perf'!A6</f>
         <v>EMP1e-EMP1w</v>
       </c>
       <c r="D17" s="3">
         <f>'raw West_perf'!B6</f>
-        <v>3.2469999999999999</v>
+        <v>3.3719999999999999</v>
       </c>
       <c r="E17" s="3">
         <f>'raw West_perf'!C6</f>
-        <v>4.13</v>
+        <v>3.7919999999999998</v>
       </c>
       <c r="F17" s="3">
         <f>'raw West_perf'!D6</f>
-        <v>4.3140000000000001</v>
+        <v>4.4619999999999997</v>
       </c>
       <c r="G17" s="3">
         <f>'raw West_perf'!E6</f>
-        <v>0.68100000000000005</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="H17" s="3">
         <f>'raw West_perf'!F6</f>
-        <v>0.875</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="I17" s="3">
         <f>'raw West_perf'!G6</f>
-        <v>0.67200000000000004</v>
+        <v>0.628</v>
       </c>
       <c r="J17" s="3">
         <f>'raw West_perf'!H6</f>
-        <v>0.32500000000000001</v>
+        <v>0.215</v>
       </c>
       <c r="K17" s="3">
         <f>'raw West_perf'!I6</f>
-        <v>0.40600000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="L17" s="3">
         <f>'raw West_perf'!J6</f>
-        <v>0.39800000000000002</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="M17" s="3">
         <f>'raw West_perf'!K6</f>
@@ -1763,49 +1766,49 @@
       </c>
       <c r="P17" s="3">
         <f>'raw West_perf'!N6</f>
-        <v>2.8260000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+        <v>1.6990000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C18" t="str">
         <f>'raw West_perf'!A7</f>
         <v>EMP2e-EMP2w</v>
       </c>
       <c r="D18" s="3">
         <f>'raw West_perf'!B7</f>
-        <v>2.4889999999999999</v>
+        <v>3.25</v>
       </c>
       <c r="E18" s="3">
         <f>'raw West_perf'!C7</f>
-        <v>2.13</v>
+        <v>3.4340000000000002</v>
       </c>
       <c r="F18" s="3">
         <f>'raw West_perf'!D7</f>
-        <v>1.5609999999999999</v>
+        <v>3.851</v>
       </c>
       <c r="G18" s="3">
         <f>'raw West_perf'!E7</f>
-        <v>0.70199999999999996</v>
+        <v>0.42099999999999999</v>
       </c>
       <c r="H18" s="3">
         <f>'raw West_perf'!F7</f>
-        <v>0.98</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="I18" s="3">
         <f>'raw West_perf'!G7</f>
-        <v>0.86899999999999999</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="J18" s="3">
         <f>'raw West_perf'!H7</f>
-        <v>0.39600000000000002</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="K18" s="3">
         <f>'raw West_perf'!I7</f>
-        <v>0.86</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="L18" s="3">
         <f>'raw West_perf'!J7</f>
-        <v>0.79300000000000004</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="M18" s="3">
         <f>'raw West_perf'!K7</f>
@@ -1821,10 +1824,10 @@
       </c>
       <c r="P18" s="3">
         <f>'raw West_perf'!N7</f>
-        <v>3.2909999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.177</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
@@ -1854,19 +1857,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G50" sqref="G50:G51"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1921,16 +1924,16 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.55400000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="F2">
-        <v>0.76</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="G2">
-        <v>0.85299999999999998</v>
+        <v>0.82099999999999995</v>
       </c>
       <c r="H2">
-        <v>0.432</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1948,39 +1951,39 @@
         <v>100</v>
       </c>
       <c r="N2">
-        <v>1.948</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.7030000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>6.024</v>
+        <v>5.8970000000000002</v>
       </c>
       <c r="C3">
-        <v>5.83</v>
+        <v>5.8970000000000002</v>
       </c>
       <c r="D3">
-        <v>5.96</v>
+        <v>5.8970000000000002</v>
       </c>
       <c r="E3">
-        <v>0.51200000000000001</v>
+        <v>0.42</v>
       </c>
       <c r="F3">
-        <v>0.66300000000000003</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="G3">
-        <v>0.72599999999999998</v>
+        <v>0.71</v>
       </c>
       <c r="H3">
-        <v>0.42199999999999999</v>
+        <v>0.316</v>
       </c>
       <c r="I3">
-        <v>0.83799999999999997</v>
+        <v>0.85</v>
       </c>
       <c r="J3">
-        <v>0.82899999999999996</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1992,39 +1995,39 @@
         <v>100</v>
       </c>
       <c r="N3">
-        <v>0.41499999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>11.991</v>
+        <v>11.792999999999999</v>
       </c>
       <c r="C4">
-        <v>11.644</v>
+        <v>11.792999999999999</v>
       </c>
       <c r="D4">
-        <v>11.91</v>
+        <v>11.792999999999999</v>
       </c>
       <c r="E4">
-        <v>0.47099999999999997</v>
+        <v>0.39</v>
       </c>
       <c r="F4">
-        <v>0.56200000000000006</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="G4">
-        <v>0.59199999999999997</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="H4">
-        <v>0.40500000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="I4">
-        <v>0.66100000000000003</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="J4">
-        <v>0.64400000000000002</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -2036,83 +2039,83 @@
         <v>100</v>
       </c>
       <c r="N4">
-        <v>0.42499999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>17.902000000000001</v>
+        <v>17.690000000000001</v>
       </c>
       <c r="C5">
-        <v>17.34</v>
+        <v>17.690000000000001</v>
       </c>
       <c r="D5">
-        <v>17.731000000000002</v>
+        <v>17.690000000000001</v>
       </c>
       <c r="E5">
-        <v>0.42899999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="F5">
-        <v>0.45900000000000002</v>
+        <v>0.434</v>
       </c>
       <c r="G5">
-        <v>0.44600000000000001</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="H5">
-        <v>0.32500000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="I5">
-        <v>0.44700000000000001</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="J5">
-        <v>0.42899999999999999</v>
+        <v>0.495</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>6.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="M5">
-        <v>99.707999999999998</v>
+        <v>99.91</v>
       </c>
       <c r="N5">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>12.595000000000001</v>
+        <v>12.279</v>
       </c>
       <c r="C6">
-        <v>14.53</v>
+        <v>15.244999999999999</v>
       </c>
       <c r="D6">
-        <v>18.193999999999999</v>
+        <v>20.606999999999999</v>
       </c>
       <c r="E6">
-        <v>0.46899999999999997</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="F6">
-        <v>0.54200000000000004</v>
+        <v>0.501</v>
       </c>
       <c r="G6">
-        <v>0.52300000000000002</v>
+        <v>0.53</v>
       </c>
       <c r="H6">
-        <v>0.28199999999999997</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="I6">
-        <v>0.34499999999999997</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="J6">
-        <v>0.33600000000000002</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2124,39 +2127,39 @@
         <v>100</v>
       </c>
       <c r="N6">
-        <v>1.9279999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
-        <v>8.6890000000000001</v>
+        <v>12.087</v>
       </c>
       <c r="C7">
-        <v>5.3630000000000004</v>
+        <v>13.739000000000001</v>
       </c>
       <c r="D7">
-        <v>3.5939999999999999</v>
+        <v>17.321999999999999</v>
       </c>
       <c r="E7">
-        <v>0.48699999999999999</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="F7">
-        <v>0.63300000000000001</v>
+        <v>0.50700000000000001</v>
       </c>
       <c r="G7">
-        <v>0.72499999999999998</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="H7">
-        <v>0.41499999999999998</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="I7">
-        <v>0.93</v>
+        <v>0.438</v>
       </c>
       <c r="J7">
-        <v>0.82299999999999995</v>
+        <v>0.438</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2168,7 +2171,7 @@
         <v>100</v>
       </c>
       <c r="N7">
-        <v>3.927</v>
+        <v>1.6519999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2177,16 +2180,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2227,7 +2230,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2241,16 +2244,16 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.80300000000000005</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="F2">
-        <v>1.1950000000000001</v>
+        <v>1.093</v>
       </c>
       <c r="G2">
-        <v>1.0760000000000001</v>
+        <v>1.081</v>
       </c>
       <c r="H2">
-        <v>0.42</v>
+        <v>0.377</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2268,39 +2271,39 @@
         <v>100</v>
       </c>
       <c r="N2">
-        <v>2.726</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.7030000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>1.6830000000000001</v>
+        <v>1.8120000000000001</v>
       </c>
       <c r="C3">
-        <v>1.8819999999999999</v>
+        <v>1.8140000000000001</v>
       </c>
       <c r="D3">
-        <v>1.752</v>
+        <v>1.8140000000000001</v>
       </c>
       <c r="E3">
-        <v>0.73899999999999999</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="F3">
-        <v>1.0369999999999999</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="G3">
-        <v>0.89500000000000002</v>
+        <v>0.876</v>
       </c>
       <c r="H3">
-        <v>0.40600000000000003</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="I3">
-        <v>0.80400000000000005</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="J3">
-        <v>0.79400000000000004</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2312,39 +2315,39 @@
         <v>100</v>
       </c>
       <c r="N3">
-        <v>1.4570000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>3.2109999999999999</v>
+        <v>3.419</v>
       </c>
       <c r="C4">
-        <v>3.7269999999999999</v>
+        <v>3.5979999999999999</v>
       </c>
       <c r="D4">
-        <v>3.3980000000000001</v>
+        <v>3.5840000000000001</v>
       </c>
       <c r="E4">
-        <v>0.68200000000000005</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="F4">
-        <v>0.89</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="G4">
-        <v>0.72399999999999998</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="H4">
-        <v>0.38600000000000001</v>
+        <v>0.318</v>
       </c>
       <c r="I4">
-        <v>0.61499999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J4">
-        <v>0.59799999999999998</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -2356,83 +2359,83 @@
         <v>100</v>
       </c>
       <c r="N4">
-        <v>1.917</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>4.5960000000000001</v>
+        <v>4.8310000000000004</v>
       </c>
       <c r="C5">
-        <v>5.3289999999999997</v>
+        <v>5.0229999999999997</v>
       </c>
       <c r="D5">
-        <v>4.7969999999999997</v>
+        <v>4.9489999999999998</v>
       </c>
       <c r="E5">
-        <v>0.628</v>
+        <v>0.378</v>
       </c>
       <c r="F5">
-        <v>0.75</v>
+        <v>0.627</v>
       </c>
       <c r="G5">
-        <v>0.56100000000000005</v>
+        <v>0.501</v>
       </c>
       <c r="H5">
-        <v>0.32100000000000001</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="I5">
-        <v>0.41899999999999998</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="J5">
-        <v>0.39900000000000002</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="M5">
-        <v>100</v>
+        <v>99.82</v>
       </c>
       <c r="N5">
-        <v>2.2549999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>3.2469999999999999</v>
+        <v>3.3719999999999999</v>
       </c>
       <c r="C6">
-        <v>4.13</v>
+        <v>3.7919999999999998</v>
       </c>
       <c r="D6">
-        <v>4.3140000000000001</v>
+        <v>4.4619999999999997</v>
       </c>
       <c r="E6">
-        <v>0.68100000000000005</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="F6">
-        <v>0.875</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="G6">
-        <v>0.67200000000000004</v>
+        <v>0.628</v>
       </c>
       <c r="H6">
-        <v>0.32500000000000001</v>
+        <v>0.215</v>
       </c>
       <c r="I6">
-        <v>0.40600000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="J6">
-        <v>0.39800000000000002</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2444,39 +2447,39 @@
         <v>100</v>
       </c>
       <c r="N6">
-        <v>2.8260000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.6990000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
-        <v>2.4889999999999999</v>
+        <v>3.25</v>
       </c>
       <c r="C7">
-        <v>2.13</v>
+        <v>3.4340000000000002</v>
       </c>
       <c r="D7">
-        <v>1.5609999999999999</v>
+        <v>3.851</v>
       </c>
       <c r="E7">
-        <v>0.70199999999999996</v>
+        <v>0.42099999999999999</v>
       </c>
       <c r="F7">
-        <v>0.98</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="G7">
-        <v>0.86899999999999999</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="H7">
-        <v>0.39600000000000002</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="I7">
-        <v>0.86</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="J7">
-        <v>0.79300000000000004</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2488,7 +2491,7 @@
         <v>100</v>
       </c>
       <c r="N7">
-        <v>3.2909999999999999</v>
+        <v>1.177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>